<commit_message>
correcion pequeña de nombres
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Maestro Muestreo de Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Maestro Muestreo de Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO/SpaOnline/ModeloDominio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="934" documentId="8_{2DE1B22A-FFC5-4559-A1FB-1A8C76F63835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFD1F89A-4984-4EFA-BFBF-EA7D8FA7C833}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4581D9-8DBB-4A71-AE43-B9412BBBF4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4815" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="7" xr2:uid="{E97E5C00-5A89-4DD9-BF1F-FD5D66024408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{E97E5C00-5A89-4DD9-BF1F-FD5D66024408}"/>
   </bookViews>
   <sheets>
     <sheet name="MaestroMuestreo" sheetId="1" r:id="rId1"/>
@@ -524,9 +524,6 @@
     <t>Notificacion de</t>
   </si>
   <si>
-    <t>Pedicura Spa-100000 - Tratamiento Facial Antiedad-120000</t>
-  </si>
-  <si>
     <t>Factura</t>
   </si>
   <si>
@@ -582,6 +579,9 @@
   </si>
   <si>
     <t>8:00 am - 18:00</t>
+  </si>
+  <si>
+    <t>Pedicura Spa-100000-Tratamiento Facial Antiedad-120000-Masaje Relajante-100000</t>
   </si>
 </sst>
 </file>
@@ -589,8 +589,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -939,10 +939,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1013,7 +1013,18 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1022,6 +1033,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1042,6 +1062,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1065,33 +1088,6 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -3138,7 +3134,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B90F74-D41C-4CC6-AFD5-8A0859489EFF}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3158,44 +3156,44 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
+      <c r="B2" s="75" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="73" t="s">
+      <c r="F3" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="72" t="s">
-        <v>163</v>
+      <c r="H3" s="51" t="s">
+        <v>162</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19">
         <v>1</v>
       </c>
@@ -3203,14 +3201,14 @@
         <v>115</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="E4" s="24" t="str">
         <f>G26 &amp;"  "&amp;G27</f>
         <v>Crema de Día Anti-edad-L'Oréal  Dermalogica Daily Microfoliant-Dermalogica</v>
       </c>
       <c r="F4" s="46">
-        <v>220000</v>
+        <v>320000</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>110</v>
@@ -3259,7 +3257,7 @@
         <v>128</v>
       </c>
       <c r="E6" s="24" t="str">
-        <f t="shared" ref="E5:E6" si="0">G28</f>
+        <f t="shared" ref="E6" si="0">G28</f>
         <v>Daily Moisture Lotion-Lubridem</v>
       </c>
       <c r="F6" s="46">
@@ -3277,11 +3275,11 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -3299,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" s="20" t="str">
         <f>C13</f>
@@ -3311,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D14" s="20" t="str">
         <f t="shared" ref="D14:D15" si="1">C14</f>
@@ -3324,7 +3322,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" s="20" t="str">
         <f t="shared" si="1"/>
@@ -3332,14 +3330,14 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
@@ -3383,7 +3381,7 @@
         <v>3:00pm-16/03/2024 Pedicura Spa-100000 Martina Corrales-1234567890</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="19">
         <v>2</v>
       </c>
@@ -3405,7 +3403,7 @@
         <v>10:00am-28/04/2024 Tratamiento Facial Antiedad-120000 Ramiro Ramirez-987654321</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="19">
         <v>3</v>
       </c>
@@ -3428,14 +3426,14 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="35" t="s">
@@ -3542,7 +3540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480D42DE-BE10-4854-BA9A-99F4B4B7DA5B}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3559,13 +3557,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
@@ -3578,7 +3576,7 @@
         <v>138</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>17</v>
@@ -3642,11 +3640,11 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3697,15 +3695,15 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
@@ -3843,11 +3841,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
@@ -3865,7 +3863,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D6" s="20" t="str">
         <f>B6&amp;" "&amp;C6</f>
@@ -3877,7 +3875,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="20" t="str">
         <f>B7&amp;" "&amp;C7</f>
@@ -3889,7 +3887,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D8" s="20" t="str">
         <f t="shared" ref="D8:D9" si="0">B8&amp;" "&amp;C8</f>
@@ -3901,7 +3899,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D9" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3943,18 +3941,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="B3" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>17</v>
@@ -3965,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" s="20" t="str">
         <f>C5</f>
@@ -3977,7 +3975,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="20" t="str">
         <f t="shared" ref="D6:D7" si="0">C6</f>
@@ -3989,7 +3987,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="20" t="str">
         <f t="shared" si="0"/>
@@ -4027,11 +4025,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -4132,7 +4130,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A9BC30-84DE-4F96-B9D6-9CF0DA2E4F6C}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4158,45 +4158,45 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="68" t="s">
+      <c r="C8" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="47" t="s">
         <v>139</v>
       </c>
       <c r="F8" s="38" t="s">
@@ -4260,7 +4260,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D11" s="19" t="str">
         <f t="shared" si="0"/>
@@ -4286,11 +4286,11 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
@@ -4350,11 +4350,11 @@
       <c r="A20" s="25"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="67"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="61"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
@@ -4443,12 +4443,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="35" t="s">
@@ -4513,14 +4513,14 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="35" t="s">
@@ -4542,7 +4542,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="21">
         <v>1</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>Dermalogica Daily Microfoliant-Dermalogica</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>3</v>
       </c>
@@ -4609,10 +4609,10 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="51"/>
+      <c r="C24" s="63"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="35" t="s">
@@ -4622,7 +4622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="21">
         <v>1</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>Dermalogica Daily Microfoliant-Dermalogica</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="21">
         <v>3</v>
       </c>
@@ -4653,16 +4653,16 @@
       <c r="C29" s="31"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="35" t="s">
@@ -4822,15 +4822,15 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
@@ -4855,7 +4855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>1</v>
       </c>
@@ -4943,14 +4943,14 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
@@ -5061,14 +5061,14 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
@@ -5084,7 +5084,7 @@
         <v>71</v>
       </c>
       <c r="F23" s="19"/>
-      <c r="G23" s="79" t="s">
+      <c r="G23" s="54" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5116,10 +5116,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>168</v>
       </c>
       <c r="E25" s="19">
         <v>1037310292</v>
@@ -5137,11 +5137,11 @@
       <c r="B26" s="19">
         <v>3</v>
       </c>
-      <c r="C26" s="78" t="s">
+      <c r="C26" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="D26" s="78" t="s">
-        <v>170</v>
       </c>
       <c r="E26" s="19">
         <v>10384182321</v>
@@ -5155,28 +5155,12 @@
         <v>Camilo Saldarriaga -salda2212</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="77"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="77"/>
-    </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
@@ -5326,17 +5310,17 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
@@ -5348,8 +5332,8 @@
       <c r="D6" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="69" t="s">
-        <v>176</v>
+      <c r="E6" s="48" t="s">
+        <v>175</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>37</v>
@@ -5382,7 +5366,7 @@
         <v>900811919-NIT-SpaOnline</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F7" s="22" t="str">
         <f>F14</f>
@@ -5418,7 +5402,7 @@
         <v>811912382-NIT-SpaManitas</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8" s="22" t="str">
         <f t="shared" ref="F8:F9" si="1">F15</f>
@@ -5454,7 +5438,7 @@
         <v>830411223-NIT-SpaOriente</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F9" s="22" t="str">
         <f t="shared" si="1"/>
@@ -5482,14 +5466,14 @@
       <c r="E10" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
@@ -5587,12 +5571,12 @@
       <c r="E18" s="40"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
@@ -5657,11 +5641,11 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
@@ -5717,15 +5701,15 @@
       <c r="D31" s="41"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
@@ -5750,7 +5734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" s="19">
         <v>1</v>
       </c>
@@ -5879,15 +5863,15 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
@@ -5991,11 +5975,11 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
@@ -6124,8 +6108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC07E9D3-5F73-4E3F-BC8B-C0E18DC9C061}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6147,14 +6131,14 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -6172,14 +6156,14 @@
       <c r="F4" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="80" t="s">
+      <c r="G4" s="55" t="s">
         <v>109</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="19">
         <v>1</v>
       </c>
@@ -6191,17 +6175,17 @@
         <v>3:00pm-16/03/2024</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="19" t="s">
         <v>110</v>
       </c>
       <c r="H5" s="23" t="str">
         <f>D5&amp;" "&amp;E5&amp;" "&amp;C5</f>
-        <v>3:00pm-16/03/2024 Pedicura Spa-100000 Martina Corrales-1234567890</v>
+        <v>3:00pm-16/03/2024 Pedicura Spa-100000-Tratamiento Facial Antiedad-120000-Masaje Relajante-100000 Martina Corrales-1234567890</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6221,7 +6205,7 @@
       <c r="F6" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="78" t="s">
+      <c r="G6" s="19" t="s">
         <v>110</v>
       </c>
       <c r="H6" s="23" t="str">
@@ -6247,7 +6231,7 @@
       <c r="F7" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="19" t="s">
         <v>110</v>
       </c>
       <c r="H7" s="23" t="str">
@@ -6256,13 +6240,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
@@ -6339,11 +6323,11 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="58" t="s">
+      <c r="B21" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
@@ -6392,16 +6376,13 @@
         <v>Masaje Relajante-100000</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="75"/>
-    </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
@@ -6466,13 +6447,13 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
@@ -6485,7 +6466,7 @@
         <v>138</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>17</v>
@@ -6549,14 +6530,14 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="17" t="s">
@@ -6642,17 +6623,17 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="17" t="s">
@@ -6783,11 +6764,11 @@
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="64" t="s">
+      <c r="B56" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="17" t="s">
@@ -6901,11 +6882,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">

</xml_diff>